<commit_message>
add new column to example data 3 tab horizontal silding of datatable without button click
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="30">
   <si>
     <t xml:space="preserve">City</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Town</t>
   </si>
   <si>
+    <t xml:space="preserve">Place</t>
+  </si>
+  <si>
     <t xml:space="preserve">Occurrence</t>
   </si>
   <si>
@@ -64,10 +67,13 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">서울시</t>
-  </si>
-  <si>
-    <t xml:space="preserve">도봉구</t>
+    <t xml:space="preserve">경기도</t>
+  </si>
+  <si>
+    <t xml:space="preserve">수원시</t>
+  </si>
+  <si>
+    <t xml:space="preserve">경기인재개발원</t>
   </si>
   <si>
     <t xml:space="preserve">김</t>
@@ -86,6 +92,12 @@
   </si>
   <si>
     <t xml:space="preserve">최</t>
+  </si>
+  <si>
+    <t xml:space="preserve">화성시</t>
+  </si>
+  <si>
+    <t xml:space="preserve">인재개발원</t>
   </si>
   <si>
     <t xml:space="preserve">정</t>
@@ -200,19 +212,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
+      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.13"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -255,1811 +268,1930 @@
       <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>16</v>
+      <c r="E2" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I2" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="0" t="n">
         <v>38.1</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="L2" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="M2" s="0" t="n">
         <v>119</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="N2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="N2" s="1" t="n">
+      <c r="O2" s="1" t="n">
         <v>43891</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>16</v>
+      <c r="E3" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I3" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="0" t="n">
         <v>36.4</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="K3" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="L3" s="0" t="n">
         <v>97</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="M3" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="N3" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="N3" s="1" t="n">
+      <c r="O3" s="1" t="n">
         <v>43890</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>16</v>
+      <c r="E4" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I4" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="0" t="n">
         <v>38.8</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="K4" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="L4" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="M4" s="0" t="n">
         <v>97</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="N4" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="N4" s="1" t="n">
+      <c r="O4" s="1" t="n">
         <v>43889</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>16</v>
+      <c r="E5" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="H5" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I5" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="0" t="n">
         <v>38.9</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="K5" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="L5" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="M5" s="0" t="n">
         <v>108</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="N5" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="N5" s="1" t="n">
+      <c r="O5" s="1" t="n">
         <v>43888</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>16</v>
+      <c r="E6" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I6" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="0" t="n">
         <v>35.9</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="K6" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="L6" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="M6" s="0" t="n">
         <v>97</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="N6" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N6" s="1" t="n">
+      <c r="O6" s="1" t="n">
         <v>43887</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>18</v>
+      <c r="E7" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I7" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="0" t="n">
         <v>36.5</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="K7" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="L7" s="0" t="n">
         <v>96</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="M7" s="0" t="n">
         <v>113</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="N7" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="N7" s="1" t="n">
+      <c r="O7" s="1" t="n">
         <v>43891</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>18</v>
+      <c r="E8" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="H8" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I8" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="K8" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="L8" s="0" t="n">
         <v>96</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="M8" s="0" t="n">
         <v>101</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="N8" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="N8" s="1" t="n">
+      <c r="O8" s="1" t="n">
         <v>43890</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>18</v>
+      <c r="E9" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="H9" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I9" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J9" s="0" t="n">
         <v>36.6</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="K9" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="L9" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="M9" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="N9" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="N9" s="1" t="n">
+      <c r="O9" s="1" t="n">
         <v>43889</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>18</v>
+      <c r="E10" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="H10" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I10" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J10" s="0" t="n">
         <v>35.5</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="K10" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="L10" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="M10" s="0" t="n">
         <v>115</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="N10" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="N10" s="1" t="n">
+      <c r="O10" s="1" t="n">
         <v>43888</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>43891</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>43891</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="N11" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>43891</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>43891</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>71</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <v>115</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="N11" s="1" t="n">
+      <c r="O11" s="1" t="n">
         <v>43887</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>19</v>
+      <c r="E12" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="H12" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I12" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="0" t="n">
         <v>37.9</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="K12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="L12" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="M12" s="0" t="n">
         <v>91</v>
       </c>
-      <c r="M12" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="N12" s="1" t="n">
+      <c r="N12" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="O12" s="1" t="n">
         <v>43891</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>19</v>
+      <c r="E13" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="H13" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I13" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="0" t="n">
         <v>38.6</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="K13" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="L13" s="0" t="n">
         <v>96</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="M13" s="0" t="n">
         <v>102</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="N13" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="N13" s="1" t="n">
+      <c r="O13" s="1" t="n">
         <v>43890</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>19</v>
+      <c r="E14" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="H14" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I14" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="0" t="n">
         <v>39.2</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="K14" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="L14" s="0" t="n">
         <v>96</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="M14" s="0" t="n">
         <v>97</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="N14" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="N14" s="1" t="n">
+      <c r="O14" s="1" t="n">
         <v>43889</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>19</v>
+      <c r="E15" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="H15" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I15" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J15" s="0" t="n">
         <v>35.1</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="K15" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="L15" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="M15" s="0" t="n">
         <v>103</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="N15" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="N15" s="1" t="n">
+      <c r="O15" s="1" t="n">
         <v>43888</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>19</v>
+      <c r="E16" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="H16" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I16" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J16" s="0" t="n">
         <v>35.9</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="K16" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="L16" s="0" t="n">
         <v>94</v>
       </c>
-      <c r="L16" s="0" t="n">
+      <c r="M16" s="0" t="n">
         <v>115</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="N16" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="N16" s="1" t="n">
+      <c r="O16" s="1" t="n">
         <v>43887</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>21</v>
+      <c r="E17" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="I17" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="J17" s="0" t="n">
         <v>35.5</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="K17" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="L17" s="0" t="n">
         <v>94</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="M17" s="0" t="n">
         <v>104</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="N17" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N17" s="1" t="n">
+      <c r="O17" s="1" t="n">
         <v>43891</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>21</v>
+      <c r="E18" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="I18" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="J18" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="K18" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="L18" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="L18" s="0" t="n">
+      <c r="M18" s="0" t="n">
         <v>91</v>
       </c>
-      <c r="M18" s="0" t="n">
+      <c r="N18" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="N18" s="1" t="n">
+      <c r="O18" s="1" t="n">
         <v>43890</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E19" s="0" t="s">
-        <v>21</v>
+      <c r="E19" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="I19" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="J19" s="0" t="n">
         <v>37.4</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="K19" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="L19" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="L19" s="0" t="n">
+      <c r="M19" s="0" t="n">
         <v>116</v>
       </c>
-      <c r="M19" s="0" t="n">
+      <c r="N19" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="N19" s="1" t="n">
+      <c r="O19" s="1" t="n">
         <v>43889</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>21</v>
+      <c r="E20" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="I20" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="J20" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="K20" s="0" t="n">
         <v>11</v>
-      </c>
-      <c r="K20" s="0" t="n">
-        <v>92</v>
       </c>
       <c r="L20" s="0" t="n">
         <v>92</v>
       </c>
       <c r="M20" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="N20" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="N20" s="1" t="n">
+      <c r="O20" s="1" t="n">
         <v>43888</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>43891</v>
+        <v>16</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>21</v>
+      <c r="E21" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="I21" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="J21" s="0" t="n">
         <v>38.2</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="K21" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="L21" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="L21" s="0" t="n">
+      <c r="M21" s="0" t="n">
         <v>108</v>
       </c>
-      <c r="M21" s="0" t="n">
+      <c r="N21" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="N21" s="1" t="n">
+      <c r="O21" s="1" t="n">
         <v>43887</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E22" s="0" t="s">
-        <v>22</v>
+      <c r="E22" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="I22" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="J22" s="0" t="n">
         <v>37.9</v>
       </c>
-      <c r="J22" s="0" t="n">
+      <c r="K22" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="L22" s="0" t="n">
         <v>96</v>
       </c>
-      <c r="L22" s="0" t="n">
+      <c r="M22" s="0" t="n">
         <v>91</v>
       </c>
-      <c r="M22" s="0" t="n">
+      <c r="N22" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="N22" s="1" t="n">
+      <c r="O22" s="1" t="n">
         <v>43891</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E23" s="0" t="s">
-        <v>22</v>
+      <c r="E23" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="I23" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="J23" s="0" t="n">
         <v>37.6</v>
       </c>
-      <c r="J23" s="0" t="n">
+      <c r="K23" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="L23" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="L23" s="0" t="n">
+      <c r="M23" s="0" t="n">
         <v>105</v>
       </c>
-      <c r="M23" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="N23" s="1" t="n">
+      <c r="N23" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="O23" s="1" t="n">
         <v>43890</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E24" s="0" t="s">
-        <v>22</v>
+      <c r="E24" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="I24" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="J24" s="0" t="n">
         <v>35.7</v>
       </c>
-      <c r="J24" s="0" t="n">
+      <c r="K24" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="L24" s="0" t="n">
         <v>94</v>
       </c>
-      <c r="L24" s="0" t="n">
+      <c r="M24" s="0" t="n">
         <v>119</v>
       </c>
-      <c r="M24" s="0" t="n">
+      <c r="N24" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="N24" s="1" t="n">
+      <c r="O24" s="1" t="n">
         <v>43889</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E25" s="0" t="s">
-        <v>22</v>
+      <c r="E25" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="I25" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="J25" s="0" t="n">
         <v>38.3</v>
       </c>
-      <c r="J25" s="0" t="n">
+      <c r="K25" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="L25" s="0" t="n">
         <v>91</v>
       </c>
-      <c r="L25" s="0" t="n">
+      <c r="M25" s="0" t="n">
         <v>94</v>
       </c>
-      <c r="M25" s="0" t="n">
+      <c r="N25" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="N25" s="1" t="n">
+      <c r="O25" s="1" t="n">
         <v>43888</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E26" s="0" t="s">
-        <v>22</v>
+      <c r="E26" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="I26" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="J26" s="0" t="n">
         <v>35.5</v>
       </c>
-      <c r="J26" s="0" t="n">
+      <c r="K26" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="K26" s="0" t="n">
+      <c r="L26" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="L26" s="0" t="n">
+      <c r="M26" s="0" t="n">
         <v>114</v>
       </c>
-      <c r="M26" s="0" t="n">
+      <c r="N26" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="N26" s="1" t="n">
+      <c r="O26" s="1" t="n">
         <v>43887</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E27" s="0" t="s">
-        <v>23</v>
+      <c r="E27" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="H27" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I27" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J27" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="J27" s="0" t="n">
+      <c r="K27" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="K27" s="0" t="n">
+      <c r="L27" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="L27" s="0" t="n">
+      <c r="M27" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="M27" s="0" t="n">
+      <c r="N27" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="N27" s="1" t="n">
+      <c r="O27" s="1" t="n">
         <v>43891</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E28" s="0" t="s">
-        <v>23</v>
+      <c r="E28" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="H28" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I28" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J28" s="0" t="n">
         <v>35.4</v>
       </c>
-      <c r="J28" s="0" t="n">
+      <c r="K28" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="K28" s="0" t="n">
+      <c r="L28" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="L28" s="0" t="n">
+      <c r="M28" s="0" t="n">
         <v>109</v>
       </c>
-      <c r="M28" s="0" t="n">
+      <c r="N28" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N28" s="1" t="n">
+      <c r="O28" s="1" t="n">
         <v>43890</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E29" s="0" t="s">
-        <v>23</v>
+      <c r="E29" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="H29" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I29" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J29" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="J29" s="0" t="n">
+      <c r="K29" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="K29" s="0" t="n">
+      <c r="L29" s="0" t="n">
         <v>96</v>
       </c>
-      <c r="L29" s="0" t="n">
+      <c r="M29" s="0" t="n">
         <v>119</v>
       </c>
-      <c r="M29" s="0" t="n">
+      <c r="N29" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="N29" s="1" t="n">
+      <c r="O29" s="1" t="n">
         <v>43889</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E30" s="0" t="s">
-        <v>23</v>
+      <c r="E30" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="H30" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I30" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J30" s="0" t="n">
         <v>38.8</v>
       </c>
-      <c r="J30" s="0" t="n">
+      <c r="K30" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="K30" s="0" t="n">
+      <c r="L30" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="L30" s="0" t="n">
+      <c r="M30" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="M30" s="0" t="n">
+      <c r="N30" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="N30" s="1" t="n">
+      <c r="O30" s="1" t="n">
         <v>43888</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E31" s="0" t="s">
-        <v>23</v>
+      <c r="E31" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="H31" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I31" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J31" s="0" t="n">
         <v>35.1</v>
       </c>
-      <c r="J31" s="0" t="n">
+      <c r="K31" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="K31" s="0" t="n">
+      <c r="L31" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="L31" s="0" t="n">
+      <c r="M31" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="M31" s="0" t="n">
+      <c r="N31" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="N31" s="1" t="n">
+      <c r="O31" s="1" t="n">
         <v>43887</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E32" s="0" t="s">
-        <v>24</v>
+      <c r="E32" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="H32" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I32" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J32" s="0" t="n">
         <v>39.5</v>
       </c>
-      <c r="J32" s="0" t="n">
+      <c r="K32" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="K32" s="0" t="n">
+      <c r="L32" s="0" t="n">
         <v>96</v>
       </c>
-      <c r="L32" s="0" t="n">
+      <c r="M32" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="M32" s="0" t="n">
+      <c r="N32" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="N32" s="1" t="n">
+      <c r="O32" s="1" t="n">
         <v>43891</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>43891</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>43891</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>39.3</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="N33" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <v>43891</v>
-      </c>
-      <c r="D33" s="1" t="n">
-        <v>43891</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="0" t="n">
-        <v>67</v>
-      </c>
-      <c r="H33" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I33" s="0" t="n">
-        <v>39.3</v>
-      </c>
-      <c r="J33" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="K33" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="L33" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="M33" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="N33" s="1" t="n">
+      <c r="O33" s="1" t="n">
         <v>43890</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E34" s="0" t="s">
-        <v>24</v>
+      <c r="E34" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="H34" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I34" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J34" s="0" t="n">
         <v>36.4</v>
       </c>
-      <c r="J34" s="0" t="n">
+      <c r="K34" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="K34" s="0" t="n">
+      <c r="L34" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="L34" s="0" t="n">
+      <c r="M34" s="0" t="n">
         <v>103</v>
       </c>
-      <c r="M34" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="N34" s="1" t="n">
+      <c r="N34" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="O34" s="1" t="n">
         <v>43889</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D35" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E35" s="0" t="s">
-        <v>24</v>
+      <c r="E35" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="H35" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I35" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J35" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="J35" s="0" t="n">
+      <c r="K35" s="0" t="n">
         <v>10</v>
-      </c>
-      <c r="K35" s="0" t="n">
-        <v>96</v>
       </c>
       <c r="L35" s="0" t="n">
         <v>96</v>
       </c>
       <c r="M35" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="N35" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="N35" s="1" t="n">
+      <c r="O35" s="1" t="n">
         <v>43888</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D36" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E36" s="0" t="s">
-        <v>24</v>
+      <c r="E36" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G36" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="H36" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="I36" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J36" s="0" t="n">
         <v>36.4</v>
       </c>
-      <c r="J36" s="0" t="n">
+      <c r="K36" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="K36" s="0" t="n">
+      <c r="L36" s="0" t="n">
         <v>91</v>
       </c>
-      <c r="L36" s="0" t="n">
+      <c r="M36" s="0" t="n">
         <v>103</v>
       </c>
-      <c r="M36" s="0" t="n">
+      <c r="N36" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="N36" s="1" t="n">
+      <c r="O36" s="1" t="n">
         <v>43887</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E37" s="0" t="s">
-        <v>25</v>
+      <c r="E37" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G37" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="H37" s="0" t="n">
+      <c r="I37" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I37" s="0" t="n">
+      <c r="J37" s="0" t="n">
         <v>36.8</v>
       </c>
-      <c r="J37" s="0" t="n">
+      <c r="K37" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="K37" s="0" t="n">
+      <c r="L37" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="L37" s="0" t="n">
+      <c r="M37" s="0" t="n">
         <v>116</v>
       </c>
-      <c r="M37" s="0" t="n">
+      <c r="N37" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="N37" s="1" t="n">
+      <c r="O37" s="1" t="n">
         <v>43891</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E38" s="0" t="s">
-        <v>25</v>
+      <c r="E38" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G38" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="H38" s="0" t="n">
+      <c r="I38" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I38" s="0" t="n">
+      <c r="J38" s="0" t="n">
         <v>35.3</v>
       </c>
-      <c r="J38" s="0" t="n">
+      <c r="K38" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="K38" s="0" t="n">
+      <c r="L38" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="L38" s="0" t="n">
+      <c r="M38" s="0" t="n">
         <v>116</v>
       </c>
-      <c r="M38" s="0" t="n">
+      <c r="N38" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="N38" s="1" t="n">
+      <c r="O38" s="1" t="n">
         <v>43890</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D39" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E39" s="0" t="s">
-        <v>25</v>
+      <c r="E39" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="H39" s="0" t="n">
+      <c r="I39" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I39" s="0" t="n">
+      <c r="J39" s="0" t="n">
         <v>35.1</v>
       </c>
-      <c r="J39" s="0" t="n">
+      <c r="K39" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="K39" s="0" t="n">
+      <c r="L39" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="L39" s="0" t="n">
+      <c r="M39" s="0" t="n">
         <v>104</v>
       </c>
-      <c r="M39" s="0" t="n">
+      <c r="N39" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N39" s="1" t="n">
+      <c r="O39" s="1" t="n">
         <v>43889</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E40" s="0" t="s">
-        <v>25</v>
+      <c r="E40" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="H40" s="0" t="n">
+      <c r="I40" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I40" s="0" t="n">
+      <c r="J40" s="0" t="n">
         <v>37.8</v>
       </c>
-      <c r="J40" s="0" t="n">
+      <c r="K40" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="K40" s="0" t="n">
+      <c r="L40" s="0" t="n">
         <v>94</v>
       </c>
-      <c r="L40" s="0" t="n">
+      <c r="M40" s="0" t="n">
         <v>114</v>
       </c>
-      <c r="M40" s="0" t="n">
+      <c r="N40" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="N40" s="1" t="n">
+      <c r="O40" s="1" t="n">
         <v>43888</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>43891</v>
+        <v>24</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>43891</v>
       </c>
-      <c r="E41" s="0" t="s">
-        <v>25</v>
+      <c r="E41" s="1" t="n">
+        <v>43891</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G41" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="H41" s="0" t="n">
+      <c r="I41" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I41" s="0" t="n">
+      <c r="J41" s="0" t="n">
         <v>37.7</v>
       </c>
-      <c r="J41" s="0" t="n">
+      <c r="K41" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="K41" s="0" t="n">
+      <c r="L41" s="0" t="n">
         <v>94</v>
       </c>
-      <c r="L41" s="0" t="n">
+      <c r="M41" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="M41" s="0" t="n">
+      <c r="N41" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="N41" s="1" t="n">
+      <c r="O41" s="1" t="n">
         <v>43887</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>